<commit_message>
descriptives: work in progress
</commit_message>
<xml_diff>
--- a/docs/efa_model_results.xlsx
+++ b/docs/efa_model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gaming\Desktop\cpa_report\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8AF135-C46E-43B5-910E-268F0A1923E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B1B33E-48B4-4FC8-B5F2-21774E0833BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Models</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>0.031  0.073</t>
+  </si>
+  <si>
+    <t>ΔRMSEA</t>
+  </si>
+  <si>
+    <t>4. Four-factor</t>
+  </si>
+  <si>
+    <t>0.000  0.028</t>
+  </si>
+  <si>
+    <t>0.000  0.047</t>
   </si>
 </sst>
 </file>
@@ -103,7 +115,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +151,19 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -208,18 +233,20 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S13"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,12 +583,14 @@
       <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="H2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -570,20 +599,20 @@
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
@@ -599,7 +628,7 @@
       <c r="B4" s="4">
         <v>54</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="15">
         <v>435.27800000000002</v>
       </c>
       <c r="D4" s="5">
@@ -614,11 +643,11 @@
       <c r="G4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
@@ -634,7 +663,7 @@
       <c r="B5" s="4">
         <v>43</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="15">
         <v>154.75700000000001</v>
       </c>
       <c r="D5" s="5">
@@ -649,11 +678,14 @@
       <c r="G5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="H5" s="10">
+        <f>F4-F5</f>
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -684,11 +716,14 @@
       <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="H6" s="10">
+        <f>F5-F6</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
       <c r="M6" s="1"/>
       <c r="N6" s="6"/>
       <c r="O6" s="1"/>
@@ -698,21 +733,36 @@
       <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="9"/>
+      <c r="A7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1">
+        <v>19.027999999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="10">
+        <f>F6-F7</f>
+        <v>0.03</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="6"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -721,34 +771,22 @@
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1">
-        <v>404.048</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.70599999999999996</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="A8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="6"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -757,31 +795,31 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1">
-        <v>128.749</v>
+        <v>44</v>
+      </c>
+      <c r="C9" s="16">
+        <v>404.048</v>
       </c>
       <c r="D9" s="1">
-        <v>0.93799999999999994</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="E9" s="1">
-        <v>0.9</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="F9" s="1">
-        <v>8.5999999999999993E-2</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+        <v>16</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -792,47 +830,103 @@
     </row>
     <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>34</v>
+      </c>
+      <c r="C10" s="16">
+        <v>128.749</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="F10" s="1">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="10">
+        <f>F9-F10</f>
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="7"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>25</v>
       </c>
-      <c r="C10">
+      <c r="C11" s="11">
         <v>50.953000000000003</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>0.98299999999999998</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>0.96299999999999997</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="H11" s="10">
+        <f>F10-F11</f>
+        <v>3.3999999999999996E-2</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="A12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>17.353999999999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="10">
+        <f>F11-F12</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
@@ -841,9 +935,16 @@
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
     </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A8:G8"/>
     <mergeCell ref="A3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>